<commit_message>
improvements here and there... mostly with number fluency app 1-20 and with the appearance of the spellingTouch app
</commit_message>
<xml_diff>
--- a/KGPS Practice - Progress & Status.xlsx
+++ b/KGPS Practice - Progress & Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Logan\Desktop\Coding Practice\KGPS Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC7EBD9-82C6-434B-87EF-09F0308479AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2B05A3-9625-4FC0-B0AF-F97308A82407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{FC6C348B-3EB7-42E1-9415-91FF75022BFA}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="21705" windowHeight="15750" activeTab="1" xr2:uid="{FC6C348B-3EB7-42E1-9415-91FF75022BFA}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
   <si>
     <t>start screen</t>
   </si>
@@ -149,6 +149,85 @@
   <si>
     <t>Found a simpler solution. Apparently I was implementing the 'white-space:nowrap' wrong… I had a dash, 'no-wrap' instead of 'nowrap'.
 I got rid of the ellipsis though, so it's more clear, and less interesting that the user has gone beyond the bounds of the letter-display.</t>
+  </si>
+  <si>
+    <t>app screen</t>
+  </si>
+  <si>
+    <t>vertical spacing is distorted on certain screens or when the viewing space is not full screen</t>
+  </si>
+  <si>
+    <t>tried media queries for height, but to no avail</t>
+  </si>
+  <si>
+    <t>app menus</t>
+  </si>
+  <si>
+    <t>no home button available to exit apps</t>
+  </si>
+  <si>
+    <t>copy over the 'exit btn' available on startup to some corner of the app</t>
+  </si>
+  <si>
+    <t>wrong answer penalty</t>
+  </si>
+  <si>
+    <t>losing points for wrong answers</t>
+  </si>
+  <si>
+    <t>have only a sound to indicate a wrong answer</t>
+  </si>
+  <si>
+    <t>the sub-menu titles were displaying directly into the top-container, leaving no room for the divs for the username and userscore</t>
+  </si>
+  <si>
+    <t>repeat button</t>
+  </si>
+  <si>
+    <t>not working</t>
+  </si>
+  <si>
+    <t>probably an orphaned div</t>
+  </si>
+  <si>
+    <t>was an orphaned div</t>
+  </si>
+  <si>
+    <t>rounds and speed</t>
+  </si>
+  <si>
+    <t>a constant speed should be kept throughout each round; that will help it feel more like a bump
+to be able to continue, you can't miss more than 5 total?</t>
+  </si>
+  <si>
+    <t>need to rearrange the rounds and the array generator</t>
+  </si>
+  <si>
+    <t>stuck on word</t>
+  </si>
+  <si>
+    <t>if a word can't be spelled correctly, can't move on to the next word</t>
+  </si>
+  <si>
+    <t>words should be skipped after a set number (3?) of tries</t>
+  </si>
+  <si>
+    <t>round change notification</t>
+  </si>
+  <si>
+    <t>it's hard to know when the round has changed</t>
+  </si>
+  <si>
+    <t>A more noticeable visible alert should do the trick, such as adding a 'wobble' effect to the round display. A more intensive alternative would be displaying an actual animated banner.</t>
+  </si>
+  <si>
+    <t>number of wrong answers display</t>
+  </si>
+  <si>
+    <t>overlaps the number buttons</t>
+  </si>
+  <si>
+    <t>need to fix the heights and positions of the different elements</t>
   </si>
 </sst>
 </file>
@@ -232,17 +311,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <strike/>
@@ -585,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9916E6F-F3FB-4EF1-A39E-A0505C5AE8F8}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -630,9 +699,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="1">
         <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -777,7 +855,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D31">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -789,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547EF13B-C0C0-4095-912E-E8B1CB1A617B}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -847,6 +925,12 @@
       <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
@@ -990,7 +1074,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D31">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1003,7 +1087,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1051,6 +1135,21 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
@@ -1194,7 +1293,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D31">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1407,7 +1506,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D31">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1419,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E960EB-B11F-4EE0-A7F5-3FFCC631CE43}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1477,25 +1576,70 @@
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="B4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="75">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="B5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="75">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="B6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45">
       <c r="A7" s="1">
         <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1620,7 +1764,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D31">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1633,7 +1777,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1710,18 +1854,39 @@
       <c r="D4" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="E4" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="F4" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="45">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="B5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30">
       <c r="A6" s="4">
         <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1851,7 +2016,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D31">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
lots of bug fixes, some new features implemented
</commit_message>
<xml_diff>
--- a/KGPS Practice - Progress & Status.xlsx
+++ b/KGPS Practice - Progress & Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Logan\Desktop\Coding Practice\KGPS Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2B05A3-9625-4FC0-B0AF-F97308A82407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D54253-254E-4A28-A33C-6C998AA37285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="21705" windowHeight="15750" activeTab="1" xr2:uid="{FC6C348B-3EB7-42E1-9415-91FF75022BFA}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="21705" windowHeight="15750" firstSheet="2" activeTab="5" xr2:uid="{FC6C348B-3EB7-42E1-9415-91FF75022BFA}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
   <si>
     <t>start screen</t>
   </si>
@@ -228,6 +228,72 @@
   </si>
   <si>
     <t>need to fix the heights and positions of the different elements</t>
+  </si>
+  <si>
+    <t>for now just added an effect on the round display</t>
+  </si>
+  <si>
+    <t>mostly taken care of… still need to be able to have responive design for vertical heights too…</t>
+  </si>
+  <si>
+    <t>2nd chances</t>
+  </si>
+  <si>
+    <t>clearing a round will now result in deletion of one of the '×' in the answer display
+however, they should probably be changed to hearts, so that users know what they're up against in the beginning?</t>
+  </si>
+  <si>
+    <t>needed extra incentive to strive for the end of a round</t>
+  </si>
+  <si>
+    <t>deletion of one of the '×' at the end of the round can provide this</t>
+  </si>
+  <si>
+    <t>number buttons</t>
+  </si>
+  <si>
+    <t>buttons can be pressed multiple times for extra points</t>
+  </si>
+  <si>
+    <t>add 'no-touch' after a number is pressed, and release it before (is this possible?) the next number is called</t>
+  </si>
+  <si>
+    <t>number speed increments between rounds</t>
+  </si>
+  <si>
+    <t>speed of numbers being called may still be too fast…</t>
+  </si>
+  <si>
+    <t>adjust intervals more
+ideally it should start becoming difficult at round 10 where point values increase</t>
+  </si>
+  <si>
+    <t>go home menu
+pause screen</t>
+  </si>
+  <si>
+    <t>blur is no strong enough to obscure what is on page, so answer can be searched for without time elapsing</t>
+  </si>
+  <si>
+    <t>Solution up and running, though currently only implemented in the number fluency app</t>
+  </si>
+  <si>
+    <t>pause button</t>
+  </si>
+  <si>
+    <t>create new FX class 'strong-blur' and use it in these situations</t>
+  </si>
+  <si>
+    <t>currently no way to directly pause when doing an activity (indirect pausing can be done using the go home button</t>
+  </si>
+  <si>
+    <t>add an icon that activates the 'pause' functionality developed for the go home feature</t>
+  </si>
+  <si>
+    <t>very strong blur</t>
+  </si>
+  <si>
+    <t>FINALLY!!!</t>
   </si>
 </sst>
 </file>
@@ -654,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9916E6F-F3FB-4EF1-A39E-A0505C5AE8F8}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -712,15 +778,45 @@
       <c r="D3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="B4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45">
       <c r="A5" s="1">
         <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -867,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547EF13B-C0C0-4095-912E-E8B1CB1A617B}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -910,6 +1006,12 @@
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45">
@@ -1519,7 +1621,8 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1627,6 +1730,12 @@
       <c r="D6" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="45">
       <c r="A7" s="1">
@@ -1641,20 +1750,59 @@
       <c r="D7" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="75">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="B8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="B9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="60">
       <c r="A10" s="1">
         <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1776,7 +1924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE81C8DC-AD59-4047-9849-BA8AF23E208B}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
1) home button functionality set for numbers app, 2) back button on main and sub menu pages fixed
</commit_message>
<xml_diff>
--- a/KGPS Practice - Progress & Status.xlsx
+++ b/KGPS Practice - Progress & Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Logan\Desktop\Coding Practice\KGPS Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D54253-254E-4A28-A33C-6C998AA37285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDF3E64-8BB8-4133-B015-B46C138D5D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="21705" windowHeight="15750" firstSheet="2" activeTab="5" xr2:uid="{FC6C348B-3EB7-42E1-9415-91FF75022BFA}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="21705" windowHeight="15750" xr2:uid="{FC6C348B-3EB7-42E1-9415-91FF75022BFA}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>audio doesn't work on iOS</t>
-  </si>
-  <si>
-    <t>polymorph… is that what it's called? Fixes are available online</t>
   </si>
   <si>
     <t>iOS audio</t>
@@ -294,6 +291,9 @@
   </si>
   <si>
     <t>FINALLY!!!</t>
+  </si>
+  <si>
+    <t>polyfill... Fixes are available online</t>
   </si>
 </sst>
 </file>
@@ -720,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9916E6F-F3FB-4EF1-A39E-A0505C5AE8F8}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -745,24 +745,24 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30">
@@ -770,19 +770,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45">
@@ -790,19 +790,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45">
@@ -810,13 +810,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -988,10 +988,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45">
@@ -1008,10 +1008,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45">
@@ -1028,10 +1028,10 @@
         <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1213,10 +1213,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30">
@@ -1238,19 +1238,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1432,10 +1432,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30">
@@ -1457,13 +1457,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1646,10 +1646,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30">
@@ -1680,7 +1680,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30">
@@ -1688,16 +1688,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="75">
@@ -1705,16 +1705,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="75">
@@ -1722,19 +1722,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45">
@@ -1742,19 +1742,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="75">
@@ -1762,19 +1762,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="45">
@@ -1782,13 +1782,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="60">
@@ -1796,13 +1796,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1924,7 +1924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE81C8DC-AD59-4047-9849-BA8AF23E208B}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1949,10 +1949,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30">
@@ -1974,19 +1974,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="225">
@@ -1994,19 +1994,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45">
@@ -2014,13 +2014,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
@@ -2028,13 +2028,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:6">

</xml_diff>

<commit_message>
added return to main menu and pause functionality, as well as fixing some layout errors
</commit_message>
<xml_diff>
--- a/KGPS Practice - Progress & Status.xlsx
+++ b/KGPS Practice - Progress & Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Logan\Desktop\Coding Practice\KGPS Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDF3E64-8BB8-4133-B015-B46C138D5D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCCE8C4-8267-4CF8-9B68-2D1D4EB633E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="21705" windowHeight="15750" xr2:uid="{FC6C348B-3EB7-42E1-9415-91FF75022BFA}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="21705" windowHeight="15750" activeTab="1" xr2:uid="{FC6C348B-3EB7-42E1-9415-91FF75022BFA}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -30,13 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
-  <si>
-    <t>start screen</t>
-  </si>
-  <si>
-    <t>x' exit button remains if start button pressed too quickly</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="93">
   <si>
     <t>Issue Location</t>
   </si>
@@ -154,9 +148,6 @@
     <t>vertical spacing is distorted on certain screens or when the viewing space is not full screen</t>
   </si>
   <si>
-    <t>tried media queries for height, but to no avail</t>
-  </si>
-  <si>
     <t>app menus</t>
   </si>
   <si>
@@ -294,13 +285,90 @@
   </si>
   <si>
     <t>polyfill... Fixes are available online</t>
+  </si>
+  <si>
+    <t>score recording</t>
+  </si>
+  <si>
+    <t>score is recorded even if the user quits in the middle of a round</t>
+  </si>
+  <si>
+    <t>the score should only be recorded if the final display container has appeared (e.g. the time is up or they have 'struck out' in a fluency activity</t>
+  </si>
+  <si>
+    <t>back button</t>
+  </si>
+  <si>
+    <t>looks amateurish</t>
+  </si>
+  <si>
+    <t>replace with an icon from font-awesome or write 'Back' or both</t>
+  </si>
+  <si>
+    <t>exit button remains if start button pressed too quickly</t>
+  </si>
+  <si>
+    <t>tried to fix it, but it may not be a timing issue?? Or the timing is wrong in another way</t>
+  </si>
+  <si>
+    <t>app start screens</t>
+  </si>
+  <si>
+    <t>round change</t>
+  </si>
+  <si>
+    <t>user can sit out entire rounds with no input</t>
+  </si>
+  <si>
+    <t>minimum requirement of at least 5-6 inputs per round, regardless of accuracy</t>
+  </si>
+  <si>
+    <t>put 'no-touch' in the answer evaluation function… if it's correct, no further input is allowed
+'no-touch' is removed before the next number is read (in the speak interval function)</t>
+  </si>
+  <si>
+    <t>home btn</t>
+  </si>
+  <si>
+    <t>weird movement when exiting app from home btn</t>
+  </si>
+  <si>
+    <t>no clue…</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tried media queries for height, but to no avail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+seems to be okay for now??</t>
+    </r>
+  </si>
+  <si>
+    <t>sorta fixed…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,6 +394,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -370,14 +446,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike/>
@@ -720,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9916E6F-F3FB-4EF1-A39E-A0505C5AE8F8}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -736,19 +822,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -756,13 +842,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30">
@@ -770,19 +856,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45">
@@ -790,19 +876,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45">
@@ -810,23 +896,47 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="60">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="B6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30">
       <c r="A7" s="1">
         <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -950,9 +1060,14 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:D31">
-    <cfRule type="expression" dxfId="5" priority="1">
+  <conditionalFormatting sqref="B2:D6 B8:D31">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>$E2="FIXED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:D7">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>$E7="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -963,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547EF13B-C0C0-4095-912E-E8B1CB1A617B}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -979,19 +1094,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45">
@@ -999,19 +1114,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45">
@@ -1019,24 +1134,39 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30">
       <c r="A4" s="1">
         <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1176,7 +1306,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D31">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1189,7 +1319,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1204,53 +1334,53 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>39</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1394,8 +1524,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:D31">
-    <cfRule type="expression" dxfId="3" priority="1">
+  <conditionalFormatting sqref="B4:D31 B2:D2">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1408,7 +1538,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1423,19 +1553,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30">
@@ -1443,27 +1573,18 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1607,9 +1728,14 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:D31">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$E2="FIXED"</formula>
+  <conditionalFormatting sqref="B4:D31">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>$E4="FIXED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:D2">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$E3="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1622,7 +1748,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1637,67 +1763,70 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="180">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="180">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="75">
@@ -1705,19 +1834,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="75">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1731,38 +1863,38 @@
         <v>52</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="75">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="75">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="60">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>60</v>
@@ -1771,13 +1903,13 @@
         <v>61</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="60">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1791,18 +1923,18 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1911,7 +2043,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:D31">
+  <conditionalFormatting sqref="B11:D31 B2:D9">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>
@@ -1925,7 +2057,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1940,41 +2072,47 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="60">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="60">
+        <v>20</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="225">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>21</v>
@@ -1983,58 +2121,49 @@
         <v>22</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="225">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="45">
+        <v>15</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30">
+        <v>45</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="4">
         <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2163,7 +2292,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:D31">
+  <conditionalFormatting sqref="B7:D31 B2:D5">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>

</xml_diff>

<commit_message>
matching app now stable and functional
</commit_message>
<xml_diff>
--- a/KGPS Practice - Progress & Status.xlsx
+++ b/KGPS Practice - Progress & Status.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Logan\Desktop\Coding Practice\KGPS Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCCE8C4-8267-4CF8-9B68-2D1D4EB633E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F1F936-7B18-475E-A117-50EE2A2CD904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="21705" windowHeight="15750" activeTab="1" xr2:uid="{FC6C348B-3EB7-42E1-9415-91FF75022BFA}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="21705" windowHeight="15750" firstSheet="2" activeTab="5" xr2:uid="{FC6C348B-3EB7-42E1-9415-91FF75022BFA}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="94">
   <si>
     <t>Issue Location</t>
   </si>
@@ -363,12 +363,15 @@
   <si>
     <t>sorta fixed…</t>
   </si>
+  <si>
+    <t>Remade the system with separate objects for start and end dots. Also implemented a hybrid observer-mediator pattern to keep track of the changes.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +411,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -429,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -449,16 +461,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <strike/>
@@ -1060,14 +1070,9 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:D6 B8:D31">
-    <cfRule type="expression" dxfId="7" priority="2">
+  <conditionalFormatting sqref="B2:D31">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$E2="FIXED"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:D7">
-    <cfRule type="expression" dxfId="6" priority="1">
-      <formula>$E7="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1078,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547EF13B-C0C0-4095-912E-E8B1CB1A617B}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1319,7 +1324,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1524,7 +1529,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B4:D31 B2:D2">
+  <conditionalFormatting sqref="B2:D2 B4:D31">
     <cfRule type="expression" dxfId="4" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>
@@ -1538,7 +1543,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1568,18 +1573,24 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30">
+    <row r="2" spans="1:6" ht="60">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="7" t="s">
         <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1728,14 +1739,14 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B4:D31">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$E4="FIXED"</formula>
+  <conditionalFormatting sqref="B2:D2">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>$E3="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:D2">
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>$E3="FIXED"</formula>
+  <conditionalFormatting sqref="B4:D31">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>$E4="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2043,7 +2054,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B11:D31 B2:D9">
+  <conditionalFormatting sqref="B2:D9 B11:D31">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>
@@ -2056,8 +2067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE81C8DC-AD59-4047-9849-BA8AF23E208B}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2292,7 +2303,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B7:D31 B2:D5">
+  <conditionalFormatting sqref="B2:D5 B7:D31">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>

</xml_diff>

<commit_message>
possible updates for mobile
</commit_message>
<xml_diff>
--- a/KGPS Practice - Progress & Status.xlsx
+++ b/KGPS Practice - Progress & Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Logan\Desktop\Coding Practice\KGPS Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F1F936-7B18-475E-A117-50EE2A2CD904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF80C492-C383-4D4F-93B2-AB650A9D5117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="21705" windowHeight="15750" firstSheet="2" activeTab="5" xr2:uid="{FC6C348B-3EB7-42E1-9415-91FF75022BFA}"/>
+    <workbookView xWindow="60" yWindow="675" windowWidth="19200" windowHeight="10350" firstSheet="1" activeTab="1" xr2:uid="{FC6C348B-3EB7-42E1-9415-91FF75022BFA}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="96">
   <si>
     <t>Issue Location</t>
   </si>
@@ -365,6 +365,12 @@
   </si>
   <si>
     <t>Remade the system with separate objects for start and end dots. Also implemented a hybrid observer-mediator pattern to keep track of the changes.</t>
+  </si>
+  <si>
+    <t>wrong answer counter</t>
+  </si>
+  <si>
+    <t>the number of the wrong answer counter does not update when the round changes and an 'x' is removed</t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547EF13B-C0C0-4095-912E-E8B1CB1A617B}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1759,7 +1765,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1948,9 +1954,18 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="45">
       <c r="A11" s="1">
         <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2067,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE81C8DC-AD59-4047-9849-BA8AF23E208B}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
minor edits to css
</commit_message>
<xml_diff>
--- a/KGPS Practice - Progress & Status.xlsx
+++ b/KGPS Practice - Progress & Status.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Logan\Desktop\Coding Practice\KGPS Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF80C492-C383-4D4F-93B2-AB650A9D5117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847BE4E6-BA28-417B-93B0-C93B89858CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="675" windowWidth="19200" windowHeight="10350" firstSheet="1" activeTab="1" xr2:uid="{FC6C348B-3EB7-42E1-9415-91FF75022BFA}"/>
+    <workbookView xWindow="0" yWindow="585" windowWidth="19200" windowHeight="13830" firstSheet="3" activeTab="3" xr2:uid="{FC6C348B-3EB7-42E1-9415-91FF75022BFA}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="106">
   <si>
     <t>Issue Location</t>
   </si>
@@ -371,6 +371,36 @@
   </si>
   <si>
     <t>the number of the wrong answer counter does not update when the round changes and an 'x' is removed</t>
+  </si>
+  <si>
+    <t>audio</t>
+  </si>
+  <si>
+    <t>text to speech default audio not very good</t>
+  </si>
+  <si>
+    <t>deciding whether to have it recorded or to use a geneartive ai solution</t>
+  </si>
+  <si>
+    <t>start AND end dot functionality</t>
+  </si>
+  <si>
+    <t>can only make lines from start dots</t>
+  </si>
+  <si>
+    <t>remade the system again… now lines can be made from start AND end dots!</t>
+  </si>
+  <si>
+    <t>media queries!</t>
+  </si>
+  <si>
+    <t>added media queries in css</t>
+  </si>
+  <si>
+    <t>different resolution screens</t>
+  </si>
+  <si>
+    <t>different res screens display app incorrectly</t>
   </si>
 </sst>
 </file>
@@ -474,7 +504,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike/>
@@ -1077,7 +1142,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D31">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1089,7 +1154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547EF13B-C0C0-4095-912E-E8B1CB1A617B}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1317,7 +1382,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D31">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1536,7 +1601,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D2 B4:D31">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1548,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B1CFA57-270E-4777-B007-718802E3C78B}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1599,14 +1664,41 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="B3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45">
       <c r="A4" s="1">
         <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1745,13 +1837,13 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:D2">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>$E3="FIXED"</formula>
+  <conditionalFormatting sqref="B2:D30">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$E2="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D31">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$E4="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1764,7 +1856,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1953,6 +2045,9 @@
       <c r="D10" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="45">
       <c r="A11" s="1">
@@ -2069,8 +2164,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:D9 B11:D31">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="B2:D31">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2083,7 +2178,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2187,9 +2282,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="30">
       <c r="A6" s="4">
         <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2319,7 +2423,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D5 B7:D31">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>$E2="FIXED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>